<commit_message>
update sql and remove data module
</commit_message>
<xml_diff>
--- a/ICustom.international.test/src/test/resources/design/国际化API.xlsx
+++ b/ICustom.international.test/src/test/resources/design/国际化API.xlsx
@@ -7,16 +7,15 @@
     <workbookView xWindow="360" yWindow="30" windowWidth="17175" windowHeight="5970"/>
   </bookViews>
   <sheets>
-    <sheet name="NavigationService-API " sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="IRegisterService-API" sheetId="4" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
+  <fileRecoveryPr autoRecover="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="47">
   <si>
     <t>接口方法名</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -34,10 +33,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>参数</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>返回</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -62,14 +57,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>services/nav/findNavigationSiteMenu</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>findNavigationSiteMenu</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>JSON</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -102,7 +89,124 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>{pageSize:20,curPage:1}</t>
+    <t>参数类型</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>P</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>参数
+[P:地址请求参数; F:表单请求参数; N:路径链接请求参数]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>N</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>String</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>findItem</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>findRecords</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>services/register/registerService/findRegisterList/10/1?regName=regName&amp;regCode=regCode&amp;regDesc=regDesc&amp;regValue=regValue</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>services/register/registerService/findRecords/10/1? classId=1&amp;className=2&amp;classCode=3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>services/register/registerService/findItem/1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>batchInsert</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>POST</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PUT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>services/international/internationalService/findLanguageList/{pageSize}/{curPage}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>services/international/internationalService/findRecords/{pageSize}/{curPage}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>services/international/internationalService/batchInsert</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>findLanguageList</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>services/international/internationalService/batchInsert</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[
+{
+"lanCode":"regCode",
+"lanValue":"描述",
+"lanType":1,
+"remarks":"0"
+}
+]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lanCode</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lanValue</t>
+  </si>
+  <si>
+    <t>lanType</t>
+  </si>
+  <si>
+    <t>remarks</t>
+  </si>
+  <si>
+    <t>services/international/internationalService/findItem/{itemId}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lanId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>i18n</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>services/international/internationalService/i18n/abc/1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>services/international/internationalService/i18n/{lanCode}/{lanType}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lanType</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -149,7 +253,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -198,24 +302,29 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
@@ -223,7 +332,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -520,180 +644,741 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B4"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="50.875" customWidth="1"/>
     <col min="4" max="4" width="18.375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.25" customWidth="1"/>
-    <col min="7" max="7" width="15.375" customWidth="1"/>
-    <col min="8" max="8" width="11.25" customWidth="1"/>
+    <col min="6" max="7" width="17.25" customWidth="1"/>
+    <col min="8" max="8" width="15.375" customWidth="1"/>
+    <col min="9" max="9" width="11.25" customWidth="1"/>
+    <col min="11" max="11" width="26.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:13" ht="33.75" customHeight="1">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="8"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="7"/>
+      <c r="K1" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:13" ht="28.5" customHeight="1">
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="15">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-    </row>
-    <row r="3" spans="1:12">
-      <c r="A3" s="3" t="s">
+      <c r="F3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" s="4"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" s="4"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" s="4"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="6"/>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" s="4"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8" s="4"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="C9" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="L9" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="M9" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" s="4"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="G10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11" s="4"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" s="4"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" s="4"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="6"/>
+      <c r="M13" s="6"/>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14" s="5"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="6"/>
+      <c r="M14" s="6"/>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="A15" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E15" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H15" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="4" t="s">
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="L15" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="M15" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="4" t="s">
+    </row>
+    <row r="16" spans="1:13">
+      <c r="A16" s="4"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="6"/>
+    </row>
+    <row r="17" spans="1:13">
+      <c r="A17" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="L17" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="5" t="s">
+      <c r="M17" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13">
+      <c r="A18" s="4"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="6"/>
+      <c r="M18" s="6"/>
+    </row>
+    <row r="19" spans="1:13">
+      <c r="A19" s="4"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G19" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="K3" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" s="4" t="s">
+      <c r="H19" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="6"/>
+      <c r="M19" s="6"/>
+    </row>
+    <row r="20" spans="1:13">
+      <c r="A20" s="4"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="6"/>
+      <c r="M20" s="6"/>
+    </row>
+    <row r="21" spans="1:13">
+      <c r="A21" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="L21" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
+      <c r="M21" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13">
+      <c r="A22" s="4"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="4"/>
+      <c r="L22" s="6"/>
+      <c r="M22" s="6"/>
+    </row>
+    <row r="23" spans="1:13">
+      <c r="A23" s="4"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="4"/>
+      <c r="L23" s="6"/>
+      <c r="M23" s="6"/>
+    </row>
+    <row r="24" spans="1:13">
+      <c r="A24" s="4"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="4"/>
+      <c r="L24" s="6"/>
+      <c r="M24" s="6"/>
+    </row>
+    <row r="25" spans="1:13">
+      <c r="A25" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="L25" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="M25" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13">
+      <c r="A26" s="9"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="9"/>
+      <c r="L26" s="6"/>
+      <c r="M26" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="18">
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="J1:J2"/>
+  <mergeCells count="58">
+    <mergeCell ref="K25:K26"/>
+    <mergeCell ref="L25:L26"/>
+    <mergeCell ref="M25:M26"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="L15:L16"/>
+    <mergeCell ref="M15:M16"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="K15:K16"/>
+    <mergeCell ref="L3:L8"/>
+    <mergeCell ref="M3:M8"/>
+    <mergeCell ref="A9:A14"/>
+    <mergeCell ref="B9:B14"/>
+    <mergeCell ref="C9:C14"/>
+    <mergeCell ref="D9:D14"/>
+    <mergeCell ref="E9:E14"/>
+    <mergeCell ref="K9:K14"/>
+    <mergeCell ref="L9:L14"/>
+    <mergeCell ref="M9:M14"/>
+    <mergeCell ref="I1:J1"/>
     <mergeCell ref="K1:K2"/>
     <mergeCell ref="L1:L2"/>
+    <mergeCell ref="M1:M2"/>
+    <mergeCell ref="A3:A8"/>
+    <mergeCell ref="B3:B8"/>
+    <mergeCell ref="C3:C8"/>
+    <mergeCell ref="D3:D8"/>
+    <mergeCell ref="E3:E8"/>
+    <mergeCell ref="K3:K8"/>
+    <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
-    <mergeCell ref="L3:L4"/>
-    <mergeCell ref="K3:K4"/>
-    <mergeCell ref="J3:J4"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="A1:A2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="K17:K20"/>
+    <mergeCell ref="L17:L20"/>
+    <mergeCell ref="M17:M20"/>
+    <mergeCell ref="A21:A24"/>
+    <mergeCell ref="B21:B24"/>
+    <mergeCell ref="C21:C24"/>
+    <mergeCell ref="D21:D24"/>
+    <mergeCell ref="E21:E24"/>
+    <mergeCell ref="K21:K24"/>
+    <mergeCell ref="L21:L24"/>
+    <mergeCell ref="M21:M24"/>
+    <mergeCell ref="A17:A20"/>
+    <mergeCell ref="B17:B20"/>
+    <mergeCell ref="C17:C20"/>
+    <mergeCell ref="D17:D20"/>
+    <mergeCell ref="E17:E20"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
-  <sheetData/>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
-  <sheetData/>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
update test documents and update Language page
</commit_message>
<xml_diff>
--- a/ICustom.international.test/src/test/resources/design/国际化API.xlsx
+++ b/ICustom.international.test/src/test/resources/design/国际化API.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="48">
   <si>
     <t>接口方法名</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -155,10 +155,6 @@
   </si>
   <si>
     <t>findLanguageList</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>services/international/internationalService/batchInsert</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -207,6 +203,14 @@
   </si>
   <si>
     <t>lanType</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>services/international/internationalService/batchUpdate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>batchUpdate</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -329,6 +333,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -338,16 +348,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -647,7 +651,7 @@
   <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+      <selection activeCell="E21" sqref="E21:E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -663,46 +667,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="33.75" customHeight="1">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="8"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7" t="s">
+      <c r="G1" s="9"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7" t="s">
+      <c r="J1" s="8"/>
+      <c r="K1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="L1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="M1" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="28.5" customHeight="1">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
       <c r="F2" s="1" t="s">
         <v>6</v>
       </c>
@@ -718,24 +722,24 @@
       <c r="J2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
     </row>
     <row r="3" spans="1:13">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="4" t="s">
         <v>10</v>
       </c>
       <c r="F3" s="2" t="s">
@@ -749,22 +753,22 @@
       </c>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
-      <c r="K3" s="3" t="s">
+      <c r="K3" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="L3" s="6" t="s">
+      <c r="L3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="M3" s="6" t="s">
+      <c r="M3" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:13">
-      <c r="A4" s="4"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
+      <c r="A4" s="6"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
       <c r="F4" s="2" t="s">
         <v>15</v>
       </c>
@@ -776,18 +780,18 @@
       </c>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
     </row>
     <row r="5" spans="1:13">
-      <c r="A5" s="4"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
+      <c r="A5" s="6"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
       <c r="F5" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>19</v>
@@ -797,18 +801,18 @@
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
     </row>
     <row r="6" spans="1:13">
-      <c r="A6" s="4"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
+      <c r="A6" s="6"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
       <c r="F6" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>19</v>
@@ -818,18 +822,18 @@
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="6"/>
-      <c r="M6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
     </row>
     <row r="7" spans="1:13">
-      <c r="A7" s="4"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
+      <c r="A7" s="6"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
       <c r="F7" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>21</v>
@@ -839,18 +843,18 @@
       </c>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="6"/>
-      <c r="M7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
     </row>
     <row r="8" spans="1:13">
-      <c r="A8" s="4"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
+      <c r="A8" s="6"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
       <c r="F8" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>21</v>
@@ -860,24 +864,24 @@
       </c>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="6"/>
-      <c r="M8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
     </row>
     <row r="9" spans="1:13">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="4" t="s">
         <v>10</v>
       </c>
       <c r="F9" s="2" t="s">
@@ -891,22 +895,22 @@
       </c>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
-      <c r="K9" s="3" t="s">
+      <c r="K9" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="L9" s="6" t="s">
+      <c r="L9" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="M9" s="6" t="s">
+      <c r="M9" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:13">
-      <c r="A10" s="4"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
+      <c r="A10" s="6"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
       <c r="F10" s="2" t="s">
         <v>15</v>
       </c>
@@ -918,18 +922,18 @@
       </c>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
-      <c r="K10" s="4"/>
-      <c r="L10" s="6"/>
-      <c r="M10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
     </row>
     <row r="11" spans="1:13">
-      <c r="A11" s="4"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
+      <c r="A11" s="6"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
       <c r="F11" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>19</v>
@@ -939,18 +943,18 @@
       </c>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
-      <c r="K11" s="4"/>
-      <c r="L11" s="6"/>
-      <c r="M11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="4"/>
+      <c r="M11" s="4"/>
     </row>
     <row r="12" spans="1:13">
-      <c r="A12" s="4"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
+      <c r="A12" s="6"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
       <c r="F12" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>19</v>
@@ -960,18 +964,18 @@
       </c>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
-      <c r="K12" s="4"/>
-      <c r="L12" s="6"/>
-      <c r="M12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
     </row>
     <row r="13" spans="1:13">
-      <c r="A13" s="4"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
+      <c r="A13" s="6"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
       <c r="F13" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>21</v>
@@ -981,18 +985,18 @@
       </c>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
-      <c r="K13" s="4"/>
-      <c r="L13" s="6"/>
-      <c r="M13" s="6"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4"/>
     </row>
     <row r="14" spans="1:13">
-      <c r="A14" s="5"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
+      <c r="A14" s="7"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
       <c r="F14" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>21</v>
@@ -1002,28 +1006,28 @@
       </c>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
-      <c r="K14" s="5"/>
-      <c r="L14" s="6"/>
-      <c r="M14" s="6"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4"/>
     </row>
     <row r="15" spans="1:13">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>42</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>19</v>
@@ -1033,49 +1037,49 @@
       </c>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
-      <c r="K15" s="3" t="s">
+      <c r="K15" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="L15" s="6" t="s">
+      <c r="L15" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="M15" s="6" t="s">
+      <c r="M15" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:13">
-      <c r="A16" s="4"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
+      <c r="A16" s="6"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
-      <c r="K16" s="4"/>
-      <c r="L16" s="6"/>
-      <c r="M16" s="6"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="4"/>
+      <c r="M16" s="4"/>
     </row>
     <row r="17" spans="1:13">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D17" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E17" s="6" t="s">
+      <c r="E17" s="4" t="s">
         <v>10</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>19</v>
@@ -1085,24 +1089,24 @@
       </c>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
-      <c r="K17" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="L17" s="6" t="s">
+      <c r="K17" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="L17" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="M17" s="6" t="s">
+      <c r="M17" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:13">
-      <c r="A18" s="4"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
+      <c r="A18" s="6"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
       <c r="F18" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>19</v>
@@ -1112,18 +1116,18 @@
       </c>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
-      <c r="K18" s="4"/>
-      <c r="L18" s="6"/>
-      <c r="M18" s="6"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="4"/>
+      <c r="M18" s="4"/>
     </row>
     <row r="19" spans="1:13">
-      <c r="A19" s="4"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
+      <c r="A19" s="6"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
       <c r="F19" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>21</v>
@@ -1133,18 +1137,18 @@
       </c>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
-      <c r="K19" s="4"/>
-      <c r="L19" s="6"/>
-      <c r="M19" s="6"/>
+      <c r="K19" s="6"/>
+      <c r="L19" s="4"/>
+      <c r="M19" s="4"/>
     </row>
     <row r="20" spans="1:13">
-      <c r="A20" s="4"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
+      <c r="A20" s="6"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
       <c r="F20" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>21</v>
@@ -1154,28 +1158,28 @@
       </c>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
-      <c r="K20" s="4"/>
-      <c r="L20" s="6"/>
-      <c r="M20" s="6"/>
+      <c r="K20" s="6"/>
+      <c r="L20" s="4"/>
+      <c r="M20" s="4"/>
     </row>
     <row r="21" spans="1:13">
-      <c r="A21" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B21" s="6" t="s">
+      <c r="A21" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B21" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C21" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D21" s="6" t="s">
+      <c r="C21" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D21" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E21" s="6" t="s">
+      <c r="E21" s="4" t="s">
         <v>10</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G21" s="2" t="s">
         <v>19</v>
@@ -1185,24 +1189,24 @@
       </c>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
-      <c r="K21" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="L21" s="6" t="s">
+      <c r="K21" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="L21" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="M21" s="6" t="s">
+      <c r="M21" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:13">
-      <c r="A22" s="4"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
+      <c r="A22" s="6"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
       <c r="F22" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G22" s="2" t="s">
         <v>19</v>
@@ -1212,18 +1216,18 @@
       </c>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
-      <c r="K22" s="4"/>
-      <c r="L22" s="6"/>
-      <c r="M22" s="6"/>
+      <c r="K22" s="6"/>
+      <c r="L22" s="4"/>
+      <c r="M22" s="4"/>
     </row>
     <row r="23" spans="1:13">
-      <c r="A23" s="4"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
+      <c r="A23" s="6"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
       <c r="F23" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G23" s="2" t="s">
         <v>21</v>
@@ -1233,18 +1237,18 @@
       </c>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
-      <c r="K23" s="4"/>
-      <c r="L23" s="6"/>
-      <c r="M23" s="6"/>
+      <c r="K23" s="6"/>
+      <c r="L23" s="4"/>
+      <c r="M23" s="4"/>
     </row>
     <row r="24" spans="1:13">
-      <c r="A24" s="4"/>
-      <c r="B24" s="6"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
+      <c r="A24" s="6"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
       <c r="F24" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G24" s="2" t="s">
         <v>21</v>
@@ -1254,28 +1258,28 @@
       </c>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
-      <c r="K24" s="4"/>
-      <c r="L24" s="6"/>
-      <c r="M24" s="6"/>
+      <c r="K24" s="6"/>
+      <c r="L24" s="4"/>
+      <c r="M24" s="4"/>
     </row>
     <row r="25" spans="1:13">
-      <c r="A25" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="B25" s="6" t="s">
+      <c r="A25" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B25" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C25" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="D25" s="6" t="s">
+      <c r="C25" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D25" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E25" s="6" t="s">
+      <c r="E25" s="4" t="s">
         <v>10</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G25" s="2" t="s">
         <v>19</v>
@@ -1285,24 +1289,24 @@
       </c>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
-      <c r="K25" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="L25" s="6" t="s">
+      <c r="K25" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="L25" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="M25" s="6" t="s">
+      <c r="M25" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="26" spans="1:13">
-      <c r="A26" s="9"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="9"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
+      <c r="A26" s="3"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
       <c r="F26" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G26" s="2" t="s">
         <v>19</v>
@@ -1312,38 +1316,28 @@
       </c>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
-      <c r="K26" s="9"/>
-      <c r="L26" s="6"/>
-      <c r="M26" s="6"/>
+      <c r="K26" s="3"/>
+      <c r="L26" s="4"/>
+      <c r="M26" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="58">
-    <mergeCell ref="K25:K26"/>
-    <mergeCell ref="L25:L26"/>
-    <mergeCell ref="M25:M26"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="L15:L16"/>
-    <mergeCell ref="M15:M16"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="K15:K16"/>
-    <mergeCell ref="L3:L8"/>
-    <mergeCell ref="M3:M8"/>
-    <mergeCell ref="A9:A14"/>
-    <mergeCell ref="B9:B14"/>
-    <mergeCell ref="C9:C14"/>
-    <mergeCell ref="D9:D14"/>
-    <mergeCell ref="E9:E14"/>
-    <mergeCell ref="K9:K14"/>
-    <mergeCell ref="L9:L14"/>
-    <mergeCell ref="M9:M14"/>
+    <mergeCell ref="K17:K20"/>
+    <mergeCell ref="L17:L20"/>
+    <mergeCell ref="M17:M20"/>
+    <mergeCell ref="A21:A24"/>
+    <mergeCell ref="B21:B24"/>
+    <mergeCell ref="C21:C24"/>
+    <mergeCell ref="D21:D24"/>
+    <mergeCell ref="E21:E24"/>
+    <mergeCell ref="K21:K24"/>
+    <mergeCell ref="L21:L24"/>
+    <mergeCell ref="M21:M24"/>
+    <mergeCell ref="A17:A20"/>
+    <mergeCell ref="B17:B20"/>
+    <mergeCell ref="C17:C20"/>
+    <mergeCell ref="D17:D20"/>
+    <mergeCell ref="E17:E20"/>
     <mergeCell ref="I1:J1"/>
     <mergeCell ref="K1:K2"/>
     <mergeCell ref="L1:L2"/>
@@ -1360,22 +1354,32 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="E1:E2"/>
     <mergeCell ref="F1:H1"/>
-    <mergeCell ref="K17:K20"/>
-    <mergeCell ref="L17:L20"/>
-    <mergeCell ref="M17:M20"/>
-    <mergeCell ref="A21:A24"/>
-    <mergeCell ref="B21:B24"/>
-    <mergeCell ref="C21:C24"/>
-    <mergeCell ref="D21:D24"/>
-    <mergeCell ref="E21:E24"/>
-    <mergeCell ref="K21:K24"/>
-    <mergeCell ref="L21:L24"/>
-    <mergeCell ref="M21:M24"/>
-    <mergeCell ref="A17:A20"/>
-    <mergeCell ref="B17:B20"/>
-    <mergeCell ref="C17:C20"/>
-    <mergeCell ref="D17:D20"/>
-    <mergeCell ref="E17:E20"/>
+    <mergeCell ref="L3:L8"/>
+    <mergeCell ref="M3:M8"/>
+    <mergeCell ref="A9:A14"/>
+    <mergeCell ref="B9:B14"/>
+    <mergeCell ref="C9:C14"/>
+    <mergeCell ref="D9:D14"/>
+    <mergeCell ref="E9:E14"/>
+    <mergeCell ref="K9:K14"/>
+    <mergeCell ref="L9:L14"/>
+    <mergeCell ref="M9:M14"/>
+    <mergeCell ref="L15:L16"/>
+    <mergeCell ref="M15:M16"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="K15:K16"/>
+    <mergeCell ref="K25:K26"/>
+    <mergeCell ref="L25:L26"/>
+    <mergeCell ref="M25:M26"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="E25:E26"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>